<commit_message>
stat individual completed (not tested thoroughly)
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/StatIndividual.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/StatIndividual.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ucs\salarizareucs\MiniPayroll\Resources\Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="9948"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,7 +359,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -465,11 +460,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -535,8 +554,24 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -546,25 +581,16 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +651,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -660,7 +686,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -837,7 +863,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -850,99 +876,99 @@
   </sheetPr>
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A2" s="30" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+    </row>
+    <row r="2" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A2" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A3" s="30" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+    </row>
+    <row r="3" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A3" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="L4" s="31" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="L4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
     </row>
     <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="L5" s="32" t="s">
+      <c r="A5" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="L5" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+    </row>
+    <row r="9" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="35"/>
+      <c r="H9" s="46"/>
       <c r="I9" s="6" t="s">
         <v>7</v>
       </c>
@@ -983,7 +1009,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1014,18 +1040,18 @@
       </c>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="36" t="s">
+      <c r="C11" s="40"/>
+      <c r="D11" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="36"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1073,12 +1099,12 @@
       </c>
       <c r="U11" s="10"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="36"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1102,7 +1128,7 @@
       <c r="T12" s="8"/>
       <c r="U12" s="10"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>43</v>
@@ -1128,10 +1154,10 @@
       <c r="I13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="42"/>
       <c r="L13" s="8" t="s">
         <v>51</v>
       </c>
@@ -1161,7 +1187,7 @@
       </c>
       <c r="U13" s="10"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
@@ -1196,14 +1222,14 @@
       <c r="T14" s="12"/>
       <c r="U14" s="10"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>1</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20">
         <v>0</v>
@@ -1211,10 +1237,10 @@
       <c r="F15" s="21">
         <v>8</v>
       </c>
-      <c r="G15" s="37">
-        <v>0</v>
-      </c>
-      <c r="H15" s="37"/>
+      <c r="G15" s="41">
+        <v>0</v>
+      </c>
+      <c r="H15" s="41"/>
       <c r="I15" s="21">
         <v>0</v>
       </c>
@@ -1254,12 +1280,12 @@
       </c>
       <c r="U15" s="22"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="30"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23">
         <v>0</v>
@@ -1313,7 +1339,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
         <v>88</v>
@@ -1372,23 +1398,23 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20">
         <f>E15</f>
         <v>0</v>
       </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="37">
+      <c r="G18" s="41">
         <f>G15</f>
         <v>0</v>
       </c>
-      <c r="H18" s="37"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="21">
         <f>I15</f>
         <v>0</v>
@@ -1437,10 +1463,10 @@
       </c>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23">
         <f>E16</f>
@@ -1503,7 +1529,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1574,39 +1600,39 @@
       <c r="U20" s="28"/>
     </row>
     <row r="22" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="38" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="38" t="s">
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="38" t="s">
+      <c r="M22" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="38" t="s">
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="R22" s="39"/>
-      <c r="S22" s="39"/>
-      <c r="T22" s="39" t="s">
+      <c r="R22" s="31"/>
+      <c r="S22" s="53"/>
+      <c r="T22" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="U22" s="34"/>
+      <c r="U22" s="37"/>
       <c r="V22" s="4"/>
     </row>
     <row r="23" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
@@ -1618,119 +1644,119 @@
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="40" t="s">
+      <c r="I23" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
       <c r="L23" s="17"/>
-      <c r="M23" s="40" t="s">
+      <c r="M23" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="41" t="s">
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="U23" s="30"/>
+      <c r="U23" s="40"/>
       <c r="V23" s="4"/>
     </row>
     <row r="24" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="44">
-        <v>0</v>
-      </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="44">
-        <v>0</v>
-      </c>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="35">
+        <v>0</v>
+      </c>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="35">
+        <v>0</v>
+      </c>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
       <c r="L24" s="17"/>
-      <c r="M24" s="38" t="s">
+      <c r="M24" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="44">
-        <v>0</v>
-      </c>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42">
-        <v>0</v>
-      </c>
-      <c r="U24" s="43"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="35">
+        <v>0</v>
+      </c>
+      <c r="R24" s="34"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="34">
+        <v>0</v>
+      </c>
+      <c r="U24" s="36"/>
       <c r="V24" s="4"/>
     </row>
     <row r="25" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="44">
-        <v>0</v>
-      </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="44">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="35">
+        <v>0</v>
+      </c>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="35">
         <f>0.0225 *E25</f>
         <v>0</v>
       </c>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
       <c r="L25" s="17"/>
-      <c r="M25" s="45" t="s">
+      <c r="M25" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="46">
-        <v>0</v>
-      </c>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
-      <c r="T25" s="42">
-        <v>0</v>
-      </c>
-      <c r="U25" s="43"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="33">
+        <v>0</v>
+      </c>
+      <c r="R25" s="51"/>
+      <c r="S25" s="52"/>
+      <c r="T25" s="34">
+        <v>0</v>
+      </c>
+      <c r="U25" s="36"/>
       <c r="V25" s="4"/>
     </row>
     <row r="26" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="44">
-        <v>0</v>
-      </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="44">
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="35">
+        <v>0</v>
+      </c>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="35">
         <f>0.3375/100*E26</f>
         <v>0</v>
       </c>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
       <c r="L26" s="17"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -1743,24 +1769,24 @@
       <c r="U26" s="1"/>
     </row>
     <row r="27" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="46">
-        <v>0</v>
-      </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="46">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="33">
         <f>0.04*E27</f>
         <v>0</v>
       </c>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
       <c r="L27" s="17"/>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
@@ -1794,78 +1820,78 @@
       <c r="T28" s="15"/>
     </row>
     <row r="29" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="38" t="s">
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="38" t="s">
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="38" t="s">
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="38" t="s">
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="38" t="s">
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
       <c r="U29" s="4"/>
     </row>
     <row r="30" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="46">
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="33">
         <f>Q15</f>
         <v>0</v>
       </c>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="46">
-        <v>0</v>
-      </c>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="46">
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="33">
         <f>Q16</f>
         <v>0</v>
       </c>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="46">
-        <v>0</v>
-      </c>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="46">
-        <v>0</v>
-      </c>
-      <c r="S30" s="42"/>
-      <c r="T30" s="42"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="33">
+        <v>0</v>
+      </c>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="33">
+        <v>0</v>
+      </c>
+      <c r="S30" s="34"/>
+      <c r="T30" s="34"/>
       <c r="U30" s="4"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1887,7 +1913,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="10.5" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>84</v>
       </c>
@@ -1898,13 +1924,60 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="I27:K27"/>
     <mergeCell ref="R29:T29"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="E30:H30"/>
@@ -1917,53 +1990,6 @@
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="L29:N29"/>
     <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
buton creeaza stat salarii pe ultimele 6 luni
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/StatIndividual.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/StatIndividual.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -555,6 +555,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -562,6 +564,10 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -585,12 +591,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,7 +877,7 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -905,70 +905,70 @@
     <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-    </row>
-    <row r="2" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="40" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-    </row>
-    <row r="3" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="40" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-    </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+    </row>
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="L4" s="43" t="s">
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="L4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-    </row>
-    <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="L5" s="44" t="s">
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+    </row>
+    <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="L5" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-    </row>
-    <row r="9" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="46" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="46"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="46"/>
+      <c r="H9" s="52"/>
       <c r="I9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1040,18 +1040,18 @@
       </c>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="42" t="s">
+      <c r="C11" s="46"/>
+      <c r="D11" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="42"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1099,12 +1099,12 @@
       </c>
       <c r="U11" s="10"/>
     </row>
-    <row r="12" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="42"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1128,7 +1128,7 @@
       <c r="T12" s="8"/>
       <c r="U12" s="10"/>
     </row>
-    <row r="13" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>43</v>
@@ -1154,10 +1154,10 @@
       <c r="I13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="42" t="s">
+      <c r="J13" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="42"/>
+      <c r="K13" s="48"/>
       <c r="L13" s="8" t="s">
         <v>51</v>
       </c>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="U13" s="10"/>
     </row>
-    <row r="14" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
@@ -1222,14 +1222,14 @@
       <c r="T14" s="12"/>
       <c r="U14" s="10"/>
     </row>
-    <row r="15" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="37"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20">
         <v>0</v>
@@ -1237,10 +1237,10 @@
       <c r="F15" s="21">
         <v>8</v>
       </c>
-      <c r="G15" s="41">
-        <v>0</v>
-      </c>
-      <c r="H15" s="41"/>
+      <c r="G15" s="47">
+        <v>0</v>
+      </c>
+      <c r="H15" s="47"/>
       <c r="I15" s="21">
         <v>0</v>
       </c>
@@ -1251,7 +1251,6 @@
         <v>0</v>
       </c>
       <c r="L15" s="20">
-        <f>E15-M15</f>
         <v>0</v>
       </c>
       <c r="M15" s="20">
@@ -1280,12 +1279,12 @@
       </c>
       <c r="U15" s="22"/>
     </row>
-    <row r="16" spans="1:21" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23">
         <v>0</v>
@@ -1339,7 +1338,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
         <v>88</v>
@@ -1398,75 +1397,77 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20">
         <f>E15</f>
         <v>0</v>
       </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="41">
+      <c r="G18" s="47">
         <f>G15</f>
         <v>0</v>
       </c>
-      <c r="H18" s="41"/>
+      <c r="H18" s="47"/>
       <c r="I18" s="21">
-        <f>I15</f>
+        <f t="shared" ref="I18:K19" si="0">I15</f>
         <v>0</v>
       </c>
       <c r="J18" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K18" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L18" s="20">
-        <f t="shared" ref="L18:T18" si="0">L15</f>
+        <f t="shared" ref="L18:T18" si="1">L15</f>
         <v>0</v>
       </c>
       <c r="M18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23">
         <f>E16</f>
@@ -1482,54 +1483,56 @@
         <v>0</v>
       </c>
       <c r="I19" s="24">
-        <f>I16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J19" s="23">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K19" s="23">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L19" s="23">
-        <f t="shared" ref="L19:T19" si="1">L16</f>
+        <f t="shared" ref="L19:T19" si="2">L16</f>
         <v>0</v>
       </c>
       <c r="M19" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N19" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O19" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P19" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q19" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R19" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S19" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T19" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1559,83 +1562,84 @@
       </c>
       <c r="J20" s="26"/>
       <c r="K20" s="26">
+        <f>K17</f>
         <v>0</v>
       </c>
       <c r="L20" s="26">
-        <f t="shared" ref="L20:T20" si="2">L17</f>
+        <f t="shared" ref="L20:T20" si="3">L17</f>
         <v>0</v>
       </c>
       <c r="M20" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N20" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O20" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P20" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q20" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R20" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S20" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T20" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U20" s="28"/>
     </row>
-    <row r="22" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="30" t="s">
+    <row r="22" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="30" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="30" t="s">
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="30" t="s">
+      <c r="M22" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="30" t="s">
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="R22" s="31"/>
-      <c r="S22" s="53"/>
-      <c r="T22" s="31" t="s">
+      <c r="R22" s="33"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="U22" s="37"/>
+      <c r="U22" s="43"/>
       <c r="V22" s="4"/>
     </row>
-    <row r="23" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1644,119 +1648,119 @@
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="38" t="s">
+      <c r="I23" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
       <c r="L23" s="17"/>
-      <c r="M23" s="38" t="s">
+      <c r="M23" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="45"/>
       <c r="Q23" s="29"/>
-      <c r="R23" s="48"/>
-      <c r="S23" s="49"/>
-      <c r="T23" s="39" t="s">
+      <c r="R23" s="30"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="U23" s="40"/>
+      <c r="U23" s="46"/>
       <c r="V23" s="4"/>
     </row>
-    <row r="24" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="35">
-        <v>0</v>
-      </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="35">
-        <v>0</v>
-      </c>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="37">
+        <v>0</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="37">
+        <v>0</v>
+      </c>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
       <c r="L24" s="17"/>
-      <c r="M24" s="30" t="s">
+      <c r="M24" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="35">
-        <v>0</v>
-      </c>
-      <c r="R24" s="34"/>
-      <c r="S24" s="50"/>
-      <c r="T24" s="34">
-        <v>0</v>
-      </c>
-      <c r="U24" s="36"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="37">
+        <v>0</v>
+      </c>
+      <c r="R24" s="36"/>
+      <c r="S24" s="41"/>
+      <c r="T24" s="36">
+        <v>0</v>
+      </c>
+      <c r="U24" s="38"/>
       <c r="V24" s="4"/>
     </row>
-    <row r="25" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="35">
-        <v>0</v>
-      </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="35">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="37">
+        <v>0</v>
+      </c>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37">
         <f>0.0225 *E25</f>
         <v>0</v>
       </c>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
       <c r="L25" s="17"/>
-      <c r="M25" s="32" t="s">
+      <c r="M25" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="33">
-        <v>0</v>
-      </c>
-      <c r="R25" s="51"/>
-      <c r="S25" s="52"/>
-      <c r="T25" s="34">
-        <v>0</v>
-      </c>
-      <c r="U25" s="36"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="35">
+        <v>0</v>
+      </c>
+      <c r="R25" s="39"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="36">
+        <v>0</v>
+      </c>
+      <c r="U25" s="38"/>
       <c r="V25" s="4"/>
     </row>
-    <row r="26" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="30" t="s">
+    <row r="26" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="35">
-        <v>0</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="35">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="37">
+        <v>0</v>
+      </c>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37">
         <f>0.3375/100*E26</f>
         <v>0</v>
       </c>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
       <c r="L26" s="17"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -1768,25 +1772,25 @@
       <c r="T26" s="16"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
+    <row r="27" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="33">
-        <v>0</v>
-      </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="33">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="35">
+        <v>0</v>
+      </c>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="35">
         <f>0.04*E27</f>
         <v>0</v>
       </c>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
       <c r="L27" s="17"/>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
@@ -1797,7 +1801,7 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1819,79 +1823,79 @@
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
     </row>
-    <row r="29" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="30" t="s">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="30" t="s">
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="30" t="s">
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="30" t="s">
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="30" t="s">
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="S29" s="31"/>
-      <c r="T29" s="31"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="33"/>
       <c r="U29" s="4"/>
     </row>
-    <row r="30" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="32" t="s">
+    <row r="30" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="33">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="35">
         <f>Q15</f>
         <v>0</v>
       </c>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="33">
-        <v>0</v>
-      </c>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="33">
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="35">
+        <v>0</v>
+      </c>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="35">
         <f>Q16</f>
         <v>0</v>
       </c>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="33">
-        <v>0</v>
-      </c>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="33">
-        <v>0</v>
-      </c>
-      <c r="S30" s="34"/>
-      <c r="T30" s="34"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="35">
+        <v>0</v>
+      </c>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="35">
+        <v>0</v>
+      </c>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
       <c r="U30" s="4"/>
     </row>
-    <row r="31" spans="1:22" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1913,7 +1917,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="36" spans="1:20" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>84</v>
       </c>
@@ -1924,7 +1928,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
fond handicap ia in calcul si zile cm
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/StatIndividual.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/StatIndividual.xlsx
@@ -557,40 +557,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,7 +863,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -877,7 +877,7 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24:K24"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -906,69 +906,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="L4" s="34" t="s">
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="L4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
     </row>
     <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="L5" s="35" t="s">
+      <c r="A5" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="L5" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="38"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="38"/>
+      <c r="H9" s="52"/>
       <c r="I9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1044,14 +1044,14 @@
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="39" t="s">
+      <c r="C11" s="46"/>
+      <c r="D11" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1154,10 +1154,10 @@
       <c r="I13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="39"/>
+      <c r="K13" s="48"/>
       <c r="L13" s="8" t="s">
         <v>51</v>
       </c>
@@ -1226,10 +1226,10 @@
       <c r="A15" s="3">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="37"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20">
         <v>0</v>
@@ -1237,10 +1237,10 @@
       <c r="F15" s="21">
         <v>8</v>
       </c>
-      <c r="G15" s="40">
-        <v>0</v>
-      </c>
-      <c r="H15" s="40"/>
+      <c r="G15" s="47">
+        <v>0</v>
+      </c>
+      <c r="H15" s="47"/>
       <c r="I15" s="21">
         <v>0</v>
       </c>
@@ -1281,10 +1281,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23">
         <v>0</v>
@@ -1399,21 +1399,21 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20">
         <f>E15</f>
         <v>0</v>
       </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="40">
+      <c r="G18" s="47">
         <f>G15</f>
         <v>0</v>
       </c>
-      <c r="H18" s="40"/>
+      <c r="H18" s="47"/>
       <c r="I18" s="21">
         <f t="shared" ref="I18:K19" si="0">I15</f>
         <v>0</v>
@@ -1466,8 +1466,8 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23">
         <f>E16</f>
@@ -1604,39 +1604,39 @@
       <c r="U20" s="28"/>
     </row>
     <row r="22" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="41" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="41" t="s">
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="41" t="s">
+      <c r="M22" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="41" t="s">
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="R22" s="42"/>
-      <c r="S22" s="43"/>
-      <c r="T22" s="42" t="s">
+      <c r="R22" s="33"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="U22" s="37"/>
+      <c r="U22" s="43"/>
       <c r="V22" s="4"/>
     </row>
     <row r="23" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
@@ -1666,102 +1666,102 @@
       <c r="T23" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="U23" s="33"/>
+      <c r="U23" s="46"/>
       <c r="V23" s="4"/>
     </row>
     <row r="24" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="48">
-        <v>0</v>
-      </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="48">
-        <v>0</v>
-      </c>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="37">
+        <v>0</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="37">
+        <v>0</v>
+      </c>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
       <c r="L24" s="17"/>
-      <c r="M24" s="41" t="s">
+      <c r="M24" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="48">
-        <v>0</v>
-      </c>
-      <c r="R24" s="46"/>
-      <c r="S24" s="53"/>
-      <c r="T24" s="46">
-        <v>0</v>
-      </c>
-      <c r="U24" s="47"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="37">
+        <v>0</v>
+      </c>
+      <c r="R24" s="36"/>
+      <c r="S24" s="41"/>
+      <c r="T24" s="36">
+        <v>0</v>
+      </c>
+      <c r="U24" s="38"/>
       <c r="V24" s="4"/>
     </row>
     <row r="25" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="48">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="37">
         <f>O19-O18-M19</f>
         <v>0</v>
       </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="48">
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37">
         <f>0.0225 *E25</f>
         <v>0</v>
       </c>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
       <c r="L25" s="17"/>
-      <c r="M25" s="49" t="s">
+      <c r="M25" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="50">
-        <v>0</v>
-      </c>
-      <c r="R25" s="51"/>
-      <c r="S25" s="52"/>
-      <c r="T25" s="46">
-        <v>0</v>
-      </c>
-      <c r="U25" s="47"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="35">
+        <v>0</v>
+      </c>
+      <c r="R25" s="39"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="36">
+        <v>0</v>
+      </c>
+      <c r="U25" s="38"/>
       <c r="V25" s="4"/>
     </row>
     <row r="26" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="48">
-        <v>0</v>
-      </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="48">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="37">
+        <v>0</v>
+      </c>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37">
         <f>0.3375/100*E26</f>
         <v>0</v>
       </c>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
       <c r="L26" s="17"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -1774,24 +1774,22 @@
       <c r="U26" s="1"/>
     </row>
     <row r="27" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="50">
-        <v>0</v>
-      </c>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="50">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="35">
         <f>0.04*E27</f>
         <v>0</v>
       </c>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
       <c r="L27" s="17"/>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
@@ -1825,75 +1823,75 @@
       <c r="T28" s="15"/>
     </row>
     <row r="29" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="41" t="s">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="41" t="s">
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="41" t="s">
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="41" t="s">
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="41" t="s">
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="33"/>
       <c r="U29" s="4"/>
     </row>
     <row r="30" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="50">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="35">
         <f>Q15</f>
         <v>0</v>
       </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="50">
-        <v>0</v>
-      </c>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="50">
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="35">
+        <v>0</v>
+      </c>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="35">
         <f>Q16</f>
         <v>0</v>
       </c>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="50">
-        <v>0</v>
-      </c>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="50">
-        <v>0</v>
-      </c>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="35">
+        <v>0</v>
+      </c>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="35">
+        <v>0</v>
+      </c>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
       <c r="U30" s="4"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -1936,6 +1934,53 @@
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="I27:K27"/>
     <mergeCell ref="R29:T29"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="E30:H30"/>
@@ -1948,53 +1993,6 @@
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="L29:N29"/>
     <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>